<commit_message>
fixing all pylint problems
</commit_message>
<xml_diff>
--- a/data_to_excel/results.xlsx
+++ b/data_to_excel/results.xlsx
@@ -28,6 +28,150 @@
     <t>Profession</t>
   </si>
   <si>
+    <t>William</t>
+  </si>
+  <si>
+    <t>Jackson</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>Student</t>
+  </si>
+  <si>
+    <t>Jennifer</t>
+  </si>
+  <si>
+    <t>Davis</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>Nurse</t>
+  </si>
+  <si>
+    <t>Elizabeth</t>
+  </si>
+  <si>
+    <t>Taylor</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>Developer</t>
+  </si>
+  <si>
+    <t>Matthew</t>
+  </si>
+  <si>
+    <t>Thompson</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>Accountant</t>
+  </si>
+  <si>
+    <t>Sarah</t>
+  </si>
+  <si>
+    <t>Smith</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>Designer</t>
+  </si>
+  <si>
+    <t>David</t>
+  </si>
+  <si>
+    <t>Brown</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>Teacher</t>
+  </si>
+  <si>
+    <t>Jessica</t>
+  </si>
+  <si>
+    <t>Miller</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>Writer</t>
+  </si>
+  <si>
+    <t>Daniel</t>
+  </si>
+  <si>
+    <t>Anderson</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>Photographer</t>
+  </si>
+  <si>
+    <t>Olivia</t>
+  </si>
+  <si>
+    <t>Lee</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>Lawyer</t>
+  </si>
+  <si>
+    <t>Emily</t>
+  </si>
+  <si>
+    <t>Williams</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>Manager</t>
+  </si>
+  <si>
+    <t>Christopher</t>
+  </si>
+  <si>
+    <t>Martinez</t>
+  </si>
+  <si>
+    <t>38</t>
+  </si>
+  <si>
+    <t>Chef</t>
+  </si>
+  <si>
+    <t>Sophia</t>
+  </si>
+  <si>
+    <t>Clark</t>
+  </si>
+  <si>
+    <t>39</t>
+  </si>
+  <si>
+    <t>Doctor</t>
+  </si>
+  <si>
     <t>Amanda</t>
   </si>
   <si>
@@ -40,102 +184,6 @@
     <t>Psychologist</t>
   </si>
   <si>
-    <t>Christopher</t>
-  </si>
-  <si>
-    <t>Martinez</t>
-  </si>
-  <si>
-    <t>38</t>
-  </si>
-  <si>
-    <t>Chef</t>
-  </si>
-  <si>
-    <t>Daniel</t>
-  </si>
-  <si>
-    <t>Anderson</t>
-  </si>
-  <si>
-    <t>33</t>
-  </si>
-  <si>
-    <t>Photographer</t>
-  </si>
-  <si>
-    <t>David</t>
-  </si>
-  <si>
-    <t>Brown</t>
-  </si>
-  <si>
-    <t>29</t>
-  </si>
-  <si>
-    <t>Teacher</t>
-  </si>
-  <si>
-    <t>Elizabeth</t>
-  </si>
-  <si>
-    <t>Taylor</t>
-  </si>
-  <si>
-    <t>26</t>
-  </si>
-  <si>
-    <t>Developer</t>
-  </si>
-  <si>
-    <t>Emily</t>
-  </si>
-  <si>
-    <t>Williams</t>
-  </si>
-  <si>
-    <t>35</t>
-  </si>
-  <si>
-    <t>Manager</t>
-  </si>
-  <si>
-    <t>Jennifer</t>
-  </si>
-  <si>
-    <t>Davis</t>
-  </si>
-  <si>
-    <t>23</t>
-  </si>
-  <si>
-    <t>Nurse</t>
-  </si>
-  <si>
-    <t>Jessica</t>
-  </si>
-  <si>
-    <t>Miller</t>
-  </si>
-  <si>
-    <t>31</t>
-  </si>
-  <si>
-    <t>Writer</t>
-  </si>
-  <si>
-    <t>Matthew</t>
-  </si>
-  <si>
-    <t>Thompson</t>
-  </si>
-  <si>
-    <t>27</t>
-  </si>
-  <si>
-    <t>Accountant</t>
-  </si>
-  <si>
     <t>Michael</t>
   </si>
   <si>
@@ -148,18 +196,6 @@
     <t>Analyst</t>
   </si>
   <si>
-    <t>Olivia</t>
-  </si>
-  <si>
-    <t>Lee</t>
-  </si>
-  <si>
-    <t>34</t>
-  </si>
-  <si>
-    <t>Lawyer</t>
-  </si>
-  <si>
     <t>Robert</t>
   </si>
   <si>
@@ -170,42 +206,6 @@
   </si>
   <si>
     <t>Architect</t>
-  </si>
-  <si>
-    <t>Sarah</t>
-  </si>
-  <si>
-    <t>Smith</t>
-  </si>
-  <si>
-    <t>28</t>
-  </si>
-  <si>
-    <t>Designer</t>
-  </si>
-  <si>
-    <t>Sophia</t>
-  </si>
-  <si>
-    <t>Clark</t>
-  </si>
-  <si>
-    <t>39</t>
-  </si>
-  <si>
-    <t>Doctor</t>
-  </si>
-  <si>
-    <t>William</t>
-  </si>
-  <si>
-    <t>Jackson</t>
-  </si>
-  <si>
-    <t>22</t>
-  </si>
-  <si>
-    <t>Student</t>
   </si>
 </sst>
 </file>
@@ -585,30 +585,30 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="2" t="s">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="2" t="s">
+      <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" t="s">
         <v>11</v>
       </c>
     </row>
@@ -711,30 +711,30 @@
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="2" t="s">
+      <c r="A11" t="s">
         <v>40</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" t="s">
         <v>42</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" t="s">
+      <c r="A12" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="2" t="s">
         <v>47</v>
       </c>
     </row>
@@ -753,16 +753,16 @@
       </c>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" t="s">
+      <c r="A14" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="2" t="s">
         <v>55</v>
       </c>
     </row>
@@ -781,16 +781,16 @@
       </c>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" t="s">
+      <c r="A16" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="2" t="s">
         <v>63</v>
       </c>
     </row>

</xml_diff>